<commit_message>
Extra testfall - problem med avrundning till heltal
</commit_message>
<xml_diff>
--- a/Blackbox-testning/Blackbox-testning.xlsx
+++ b/Blackbox-testning/Blackbox-testning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Testfall nummer</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>Förbättra programlogiken och introducera felhantering</t>
+  </si>
+  <si>
+    <t>Giltig triangel med sidor där decimaltalet börjar på samma heltal</t>
+  </si>
+  <si>
+    <t>1,2 1,3 1,4</t>
+  </si>
+  <si>
+    <t>Applikationen avrundar double värden till heltal, därmed blir resultatet ej korrekt (testfall 11)</t>
   </si>
 </sst>
 </file>
@@ -493,13 +502,13 @@
   <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.42578125" customWidth="1"/>
@@ -716,6 +725,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>33</v>
@@ -729,6 +758,11 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
uppdat blackbox doc, ny clean sulution med 10 unittests
</commit_message>
<xml_diff>
--- a/Blackbox-testning/Blackbox-testning.xlsx
+++ b/Blackbox-testning/Blackbox-testning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Testfall nummer</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>Applikationen avrundar double värden till heltal, därmed blir resultatet ej korrekt (testfall 11)</t>
+  </si>
+  <si>
+    <t>Likbent triangel där lika sidor kommer sist som inparametrar</t>
+  </si>
+  <si>
+    <t>4,2 3 3</t>
+  </si>
+  <si>
+    <t>Testomgång1</t>
+  </si>
+  <si>
+    <t>En inparameter ej giltig/ej double</t>
+  </si>
+  <si>
+    <t>4,2 3 ett</t>
   </si>
 </sst>
 </file>
@@ -499,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +529,11 @@
     <col min="6" max="6" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -745,33 +765,70 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>